<commit_message>
feat: agregar scripts UFT y recursos actualizados
</commit_message>
<xml_diff>
--- a/DemoLoginPSL/Default.xlsx
+++ b/DemoLoginPSL/Default.xlsx
@@ -177,7 +177,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -188,9 +190,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -205,11 +205,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,37 +509,38 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="23.0078125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.48828125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="14.95" s="2" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>701470069</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>110220326</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>207110407</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>503550532</v>
       </c>
     </row>
@@ -556,12 +557,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -580,7 +581,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -599,7 +600,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>